<commit_message>
add section 5 to rhesults of Oct 2015
</commit_message>
<xml_diff>
--- a/files/QT/Exam_Oct_2015_results.xlsx
+++ b/files/QT/Exam_Oct_2015_results.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" tabRatio="500"/>
+    <workbookView xWindow="12800" yWindow="0" windowWidth="12800" windowHeight="15480" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Section 1" sheetId="1" r:id="rId1"/>
     <sheet name="Section 2" sheetId="2" r:id="rId2"/>
     <sheet name="Section 3" sheetId="4" r:id="rId3"/>
     <sheet name="Section 4" sheetId="5" r:id="rId4"/>
+    <sheet name="Section 5" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="62">
   <si>
     <t>Year</t>
   </si>
@@ -227,6 +228,36 @@
   <si>
     <t>$/€</t>
   </si>
+  <si>
+    <t>Wages</t>
+  </si>
+  <si>
+    <t>Frequency</t>
+  </si>
+  <si>
+    <t>1k - 2k</t>
+  </si>
+  <si>
+    <t>2k - 3k</t>
+  </si>
+  <si>
+    <t>3k - 4k</t>
+  </si>
+  <si>
+    <t>4k - 5k</t>
+  </si>
+  <si>
+    <t>1. What is the modal class ?</t>
+  </si>
+  <si>
+    <t>Cumulative Frequencies</t>
+  </si>
+  <si>
+    <t>2. What is the median class ?</t>
+  </si>
+  <si>
+    <t>The median is the wage of the 9 employee which belongs to the class 3k - 4k</t>
+  </si>
 </sst>
 </file>
 
@@ -238,13 +269,12 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="0.0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -295,6 +325,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -438,7 +475,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="83">
+  <cellStyleXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -522,8 +559,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -652,8 +691,16 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="83">
+  <cellStyles count="85">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -695,6 +742,7 @@
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -736,6 +784,7 @@
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1067,7 +1116,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+    <sheetView topLeftCell="A5" workbookViewId="0">
       <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
@@ -1791,4 +1840,108 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="2" spans="1:3">
+      <c r="A2" s="54" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="54" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="55" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="1">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <f>B3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <f>B4+C3</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B5" s="1">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:C6" si="0">B5+C4</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="1">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B8" s="57"/>
+      <c r="C8" s="57"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="56" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="57"/>
+      <c r="C10" s="57"/>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>61</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>